<commit_message>
0.0.5: Enable spacifying line separator code.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtTask.xlsx
+++ b/meta/program/BlancoValueObjectKtTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA2DBB5-E257-C240-B385-25CAFB6C9859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999550D4-CC1D-9344-A08C-103465074612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,12 +27,22 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">config!$C$5:$C$6</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -270,6 +280,24 @@
   </si>
   <si>
     <t>バリューオブジェクト定義書からソースコードを自動生成する BlancoValueObjectKtのAntTaskです。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>lineSeparator</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>LF</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>行末記号をしていします。LF=0x0a, CR=0x0d, CFLF=0x0d0x0a とします。LFがデフォルトです。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ギョウマツ </t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t xml:space="preserve">キゴウヲ </t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -737,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -845,6 +873,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -880,15 +918,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1258,10 +1296,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1307,10 +1345,10 @@
       <c r="F5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="76"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="6" t="s">
         <v>43</v>
       </c>
@@ -1320,10 +1358,10 @@
       <c r="G6" s="36"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="76"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="6" t="s">
         <v>44</v>
       </c>
@@ -1334,10 +1372,10 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="76"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="6" t="s">
         <v>45</v>
       </c>
@@ -1348,10 +1386,10 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="76"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="11" t="s">
         <v>7</v>
       </c>
@@ -1383,38 +1421,38 @@
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
-      <c r="A12" s="72" t="s">
+      <c r="A12" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="74" t="s">
+      <c r="D12" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="75" t="s">
+      <c r="E12" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="F12" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="72"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
     </row>
     <row r="14" spans="1:9" ht="27" customHeight="1">
       <c r="A14" s="44">
@@ -1430,12 +1468,12 @@
         <v>13</v>
       </c>
       <c r="E14" s="48"/>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="66"/>
     </row>
     <row r="15" spans="1:9" ht="27" customHeight="1">
       <c r="A15" s="49">
@@ -1451,12 +1489,12 @@
       <c r="E15" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="66" t="s">
+      <c r="F15" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="68"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="72"/>
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1">
       <c r="A16" s="49">
@@ -1472,12 +1510,12 @@
       <c r="E16" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="69" t="s">
+      <c r="F16" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="68"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="72"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="49">
@@ -1554,23 +1592,34 @@
       <c r="E20" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="63" t="s">
+      <c r="F20" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="65"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="42"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="69"/>
+    </row>
+    <row r="21" spans="1:9" ht="52" customHeight="1">
+      <c r="A21" s="49">
+        <f t="shared" ref="A21" si="0">A20+1</f>
+        <v>8</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>17</v>
+      </c>
       <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
+      <c r="E21" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="81" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="83"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="22"/>
@@ -1617,23 +1666,30 @@
       <c r="I25" s="27"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="33"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F14:I14"/>
+  <mergeCells count="15">
+    <mergeCell ref="F21:I21"/>
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
@@ -1643,17 +1699,22 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F42" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F43" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D26" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D20 D22:D27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C26" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C20 C22:C27" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>